<commit_message>
Updated Matched,Files from s3
</commit_message>
<xml_diff>
--- a/llm_invoice_reconciliation.xlsx
+++ b/llm_invoice_reconciliation.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,77 +441,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>amount</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
+          <t>info</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-06-22</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>27033.29</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ACH Payment - Omkar Mestry INV-20250620-996A7766</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-06-21</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>28518.85</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ACH Payment - Global Mfg Corp INV-20250620-D0E0F066</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-06-22</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>27033.29</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ACH Payment - Omkar Mestry INV-20250620-996A7766</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-06-21</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>28518.85</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ACH Payment - Global Mfg Corp INV-20250620-D0E0F066</t>
+          <t>No data</t>
         </is>
       </c>
     </row>
@@ -526,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,15 +474,48 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>info</t>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>amount</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>No data</t>
-        </is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Invoice INV-20250623-59B50E89</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>28518.85</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Invoice INV-20250623-9406A583</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>27033.29</v>
       </c>
     </row>
   </sheetData>
@@ -559,7 +529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -597,19 +567,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-06-23</t>
+          <t>2025-06-21</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Monthly Office Rent Brightspace Realty</t>
+          <t>ACH Payment - Global Mfg Corp INV-20250620-D0E0F066</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4000</v>
+        <v>28518.85</v>
       </c>
       <c r="D2" t="n">
-        <v>176552.14</v>
+        <v>153518.85</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -620,19 +590,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-06-24</t>
+          <t>2025-06-22</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Software Subscription - Adobe SuiteAdobe Inc.</t>
+          <t>ACH Payment - Omkar Mestry INV-20250620-996A7766</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>189.99</v>
+        <v>27033.29</v>
       </c>
       <c r="D3" t="n">
-        <v>176362.15</v>
+        <v>180552.14</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -643,19 +613,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-06-25</t>
+          <t>2025-06-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Internet Bill FastNet Communications</t>
+          <t>Monthly Office Rent Brightspace Realty</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>79.98999999999999</v>
+        <v>4000</v>
       </c>
       <c r="D4" t="n">
-        <v>176282.16</v>
+        <v>176552.14</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -666,19 +636,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-06-26</t>
+          <t>2025-06-24</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Employee Salary - June Payroll Transfer</t>
+          <t>Software Subscription - Adobe SuiteAdobe Inc.</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>55000</v>
+        <v>189.99</v>
       </c>
       <c r="D5" t="n">
-        <v>121282.16</v>
+        <v>176362.15</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -689,19 +659,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-06-27</t>
+          <t>2025-06-25</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Utility Payment - Electricity City Utilities</t>
+          <t>Internet Bill FastNet Communications</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>750</v>
+        <v>79.98999999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>120532.16</v>
+        <v>176282.16</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -712,19 +682,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-06-28</t>
+          <t>2025-06-26</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Payment from TechDynamics LLC Invoice INV-TD-1234</t>
+          <t>Employee Salary - June Payroll Transfer</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>18750</v>
+        <v>55000</v>
       </c>
       <c r="D7" t="n">
-        <v>139282.16</v>
+        <v>121282.16</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -735,21 +705,67 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>2025-06-27</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Utility Payment - Electricity City Utilities</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>750</v>
+      </c>
+      <c r="D8" t="n">
+        <v>120532.16</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>credit</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-06-28</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Payment from TechDynamics LLC Invoice INV-TD-1234</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>18750</v>
+      </c>
+      <c r="D9" t="n">
+        <v>139282.16</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>credit</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>2025-06-29</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Amazon Business Purchase Amazon.com</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C10" t="n">
         <v>320.5</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D10" t="n">
         <v>138961.66</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>credit</t>
         </is>

</xml_diff>

<commit_message>
Changed to old code
</commit_message>
<xml_diff>
--- a/llm_invoice_reconciliation.xlsx
+++ b/llm_invoice_reconciliation.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,48 +474,15 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>amount</t>
+          <t>info</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-06-23</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Invoice INV-20250623-59B50E89</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>28518.85</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-06-23</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Invoice INV-20250623-9406A583</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>27033.29</v>
+          <t>No data</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -529,7 +496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,234 +507,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>amount</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>balance</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>type</t>
+          <t>info</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-06-21</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ACH Payment - Global Mfg Corp INV-20250620-D0E0F066</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>28518.85</v>
-      </c>
-      <c r="D2" t="n">
-        <v>153518.85</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>credit</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-06-22</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ACH Payment - Omkar Mestry INV-20250620-996A7766</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>27033.29</v>
-      </c>
-      <c r="D3" t="n">
-        <v>180552.14</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>credit</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-06-23</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Monthly Office Rent Brightspace Realty</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D4" t="n">
-        <v>176552.14</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>credit</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-06-24</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Software Subscription - Adobe SuiteAdobe Inc.</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>189.99</v>
-      </c>
-      <c r="D5" t="n">
-        <v>176362.15</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>credit</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-06-25</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Internet Bill FastNet Communications</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>79.98999999999999</v>
-      </c>
-      <c r="D6" t="n">
-        <v>176282.16</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>credit</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-06-26</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Employee Salary - June Payroll Transfer</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>55000</v>
-      </c>
-      <c r="D7" t="n">
-        <v>121282.16</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>credit</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-06-27</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Utility Payment - Electricity City Utilities</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>750</v>
-      </c>
-      <c r="D8" t="n">
-        <v>120532.16</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>credit</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-06-28</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Payment from TechDynamics LLC Invoice INV-TD-1234</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>18750</v>
-      </c>
-      <c r="D9" t="n">
-        <v>139282.16</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>credit</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2025-06-29</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Amazon Business Purchase Amazon.com</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>320.5</v>
-      </c>
-      <c r="D10" t="n">
-        <v>138961.66</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>credit</t>
+          <t>No data</t>
         </is>
       </c>
     </row>

</xml_diff>